<commit_message>
created command line py
</commit_message>
<xml_diff>
--- a/tests/xls/BOM_1.xlsx
+++ b/tests/xls/BOM_1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1920" yWindow="1920" windowWidth="18600" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BOM" sheetId="1" state="visible" r:id="rId1"/>
@@ -425,7 +425,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
highlight missing items, still problems with grey
</commit_message>
<xml_diff>
--- a/tests/xls/BOM_1.xlsx
+++ b/tests/xls/BOM_1.xlsx
@@ -2628,11 +2628,23 @@
       <c r="AH37" s="13" t="n"/>
     </row>
     <row r="38" ht="14.4" customHeight="1">
-      <c r="A38" s="8" t="n"/>
-      <c r="B38" s="8" t="n"/>
-      <c r="C38" s="8" t="n"/>
-      <c r="D38" s="8" t="n"/>
-      <c r="E38" s="12" t="n"/>
+      <c r="A38" s="8" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8" t="inlineStr">
+        <is>
+          <t>HE</t>
+        </is>
+      </c>
+      <c r="C38" s="8" t="n">
+        <v>905</v>
+      </c>
+      <c r="D38" s="8" t="inlineStr"/>
+      <c r="E38" s="12" t="inlineStr">
+        <is>
+          <t>HE905</t>
+        </is>
+      </c>
       <c r="F38" s="8" t="n"/>
       <c r="G38" s="8" t="n"/>
       <c r="H38" s="8" t="n"/>
@@ -2640,8 +2652,16 @@
       <c r="J38" s="8" t="n"/>
       <c r="K38" s="8" t="n"/>
       <c r="L38" s="8" t="n"/>
-      <c r="M38" s="9" t="n"/>
-      <c r="N38" s="9" t="n"/>
+      <c r="M38" s="9" t="inlineStr">
+        <is>
+          <t>Heater Exchanger</t>
+        </is>
+      </c>
+      <c r="N38" s="9" t="inlineStr">
+        <is>
+          <t>Heater Exchanger</t>
+        </is>
+      </c>
       <c r="O38" s="8" t="n"/>
       <c r="P38" s="9" t="n"/>
       <c r="Q38" s="10" t="n"/>

</xml_diff>

<commit_message>
added C type + corrected valve search type
</commit_message>
<xml_diff>
--- a/tests/xls/BOM_1.xlsx
+++ b/tests/xls/BOM_1.xlsx
@@ -679,12 +679,12 @@
         </is>
       </c>
       <c r="C2" s="8" t="n">
-        <v>910</v>
+        <v>905</v>
       </c>
       <c r="D2" s="8" t="inlineStr"/>
       <c r="E2" s="12" t="inlineStr">
         <is>
-          <t>CH910</t>
+          <t>CH905</t>
         </is>
       </c>
       <c r="F2" s="8" t="n"/>
@@ -731,16 +731,16 @@
       </c>
       <c r="B3" s="8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>CH</t>
         </is>
       </c>
       <c r="C3" s="8" t="n">
-        <v>100</v>
+        <v>910</v>
       </c>
       <c r="D3" s="8" t="inlineStr"/>
       <c r="E3" s="12" t="inlineStr">
         <is>
-          <t>D100</t>
+          <t>CH910</t>
         </is>
       </c>
       <c r="F3" s="8" t="n"/>
@@ -752,12 +752,12 @@
       <c r="L3" s="8" t="n"/>
       <c r="M3" s="9" t="inlineStr">
         <is>
-          <t>Tank</t>
+          <t>Chiller</t>
         </is>
       </c>
       <c r="N3" s="9" t="inlineStr">
         <is>
-          <t>Vasca Satinatura</t>
+          <t>Chiller</t>
         </is>
       </c>
       <c r="O3" s="8" t="n"/>
@@ -791,12 +791,12 @@
         </is>
       </c>
       <c r="C4" s="8" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D4" s="8" t="inlineStr"/>
       <c r="E4" s="12" t="inlineStr">
         <is>
-          <t>D200</t>
+          <t>D100</t>
         </is>
       </c>
       <c r="F4" s="8" t="n"/>
@@ -813,7 +813,7 @@
       </c>
       <c r="N4" s="9" t="inlineStr">
         <is>
-          <t>Vasca Stoccaggio</t>
+          <t>Vasca Satinatura</t>
         </is>
       </c>
       <c r="O4" s="8" t="n"/>
@@ -847,12 +847,12 @@
         </is>
       </c>
       <c r="C5" s="8" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="D5" s="8" t="inlineStr"/>
       <c r="E5" s="12" t="inlineStr">
         <is>
-          <t>D500</t>
+          <t>D200</t>
         </is>
       </c>
       <c r="F5" s="8" t="n"/>
@@ -903,12 +903,12 @@
         </is>
       </c>
       <c r="C6" s="8" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="D6" s="8" t="inlineStr"/>
       <c r="E6" s="12" t="inlineStr">
         <is>
-          <t>D700</t>
+          <t>D500</t>
         </is>
       </c>
       <c r="F6" s="8" t="n"/>
@@ -925,7 +925,7 @@
       </c>
       <c r="N6" s="9" t="inlineStr">
         <is>
-          <t>Serbatoi stoccaggio</t>
+          <t>Vasca Stoccaggio</t>
         </is>
       </c>
       <c r="O6" s="8" t="n"/>
@@ -959,12 +959,12 @@
         </is>
       </c>
       <c r="C7" s="8" t="n">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="D7" s="8" t="inlineStr"/>
       <c r="E7" s="12" t="inlineStr">
         <is>
-          <t>D800</t>
+          <t>D700</t>
         </is>
       </c>
       <c r="F7" s="8" t="n"/>
@@ -981,7 +981,7 @@
       </c>
       <c r="N7" s="9" t="inlineStr">
         <is>
-          <t>Serbatoio di refluo contenente ammoniaca</t>
+          <t>Serbatoi stoccaggio</t>
         </is>
       </c>
       <c r="O7" s="8" t="n"/>
@@ -1015,12 +1015,12 @@
         </is>
       </c>
       <c r="C8" s="8" t="n">
-        <v>850</v>
+        <v>800</v>
       </c>
       <c r="D8" s="8" t="inlineStr"/>
       <c r="E8" s="12" t="inlineStr">
         <is>
-          <t>D850</t>
+          <t>D800</t>
         </is>
       </c>
       <c r="F8" s="8" t="n"/>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="N8" s="9" t="inlineStr">
         <is>
-          <t>Torre di strippaggio</t>
+          <t>Serbatoio di refluo contenente ammoniaca</t>
         </is>
       </c>
       <c r="O8" s="8" t="n"/>
@@ -1067,18 +1067,16 @@
       </c>
       <c r="B9" s="8" t="inlineStr">
         <is>
-          <t>FT</t>
+          <t>D</t>
         </is>
       </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>501</t>
-        </is>
+      <c r="C9" s="8" t="n">
+        <v>850</v>
       </c>
       <c r="D9" s="8" t="inlineStr"/>
       <c r="E9" s="12" t="inlineStr">
         <is>
-          <t>FT501</t>
+          <t>D850</t>
         </is>
       </c>
       <c r="F9" s="8" t="n"/>
@@ -1090,10 +1088,14 @@
       <c r="L9" s="8" t="n"/>
       <c r="M9" s="9" t="inlineStr">
         <is>
-          <t>Flowmeter Impulse</t>
+          <t>Tank</t>
         </is>
       </c>
-      <c r="N9" s="9" t="n"/>
+      <c r="N9" s="9" t="inlineStr">
+        <is>
+          <t>Torre di strippaggio</t>
+        </is>
+      </c>
       <c r="O9" s="8" t="n"/>
       <c r="P9" s="9" t="n"/>
       <c r="Q9" s="10" t="n"/>
@@ -1121,16 +1123,18 @@
       </c>
       <c r="B10" s="8" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>FT</t>
         </is>
       </c>
-      <c r="C10" s="8" t="n">
-        <v>200</v>
+      <c r="C10" s="8" t="inlineStr">
+        <is>
+          <t>501</t>
+        </is>
       </c>
       <c r="D10" s="8" t="inlineStr"/>
       <c r="E10" s="12" t="inlineStr">
         <is>
-          <t>G200</t>
+          <t>FT501</t>
         </is>
       </c>
       <c r="F10" s="8" t="n"/>
@@ -1142,14 +1146,10 @@
       <c r="L10" s="8" t="n"/>
       <c r="M10" s="9" t="inlineStr">
         <is>
-          <t>Pompa</t>
+          <t>Flowmeter Impulse</t>
         </is>
       </c>
-      <c r="N10" s="9" t="inlineStr">
-        <is>
-          <t>Pompa a Cavità progressiva</t>
-        </is>
-      </c>
+      <c r="N10" s="9" t="n"/>
       <c r="O10" s="8" t="n"/>
       <c r="P10" s="9" t="n"/>
       <c r="Q10" s="10" t="n"/>
@@ -1181,12 +1181,12 @@
         </is>
       </c>
       <c r="C11" s="8" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D11" s="8" t="inlineStr"/>
       <c r="E11" s="12" t="inlineStr">
         <is>
-          <t>G300</t>
+          <t>G200</t>
         </is>
       </c>
       <c r="F11" s="8" t="n"/>
@@ -1198,12 +1198,12 @@
       <c r="L11" s="8" t="n"/>
       <c r="M11" s="9" t="inlineStr">
         <is>
-          <t>FiltroPressa</t>
+          <t>Pompa</t>
         </is>
       </c>
       <c r="N11" s="9" t="inlineStr">
         <is>
-          <t>Filtropressa</t>
+          <t>Pompa a Cavità progressiva</t>
         </is>
       </c>
       <c r="O11" s="8" t="n"/>
@@ -1237,12 +1237,12 @@
         </is>
       </c>
       <c r="C12" s="8" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D12" s="8" t="inlineStr"/>
       <c r="E12" s="12" t="inlineStr">
         <is>
-          <t>G400</t>
+          <t>G300</t>
         </is>
       </c>
       <c r="F12" s="8" t="n"/>
@@ -1254,12 +1254,12 @@
       <c r="L12" s="8" t="n"/>
       <c r="M12" s="9" t="inlineStr">
         <is>
-          <t>Screw Conveyor</t>
+          <t>FiltroPressa</t>
         </is>
       </c>
       <c r="N12" s="9" t="inlineStr">
         <is>
-          <t>Screw Conveyor</t>
+          <t>Filtropressa</t>
         </is>
       </c>
       <c r="O12" s="8" t="n"/>
@@ -1293,12 +1293,12 @@
         </is>
       </c>
       <c r="C13" s="8" t="n">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="D13" s="8" t="inlineStr"/>
       <c r="E13" s="12" t="inlineStr">
         <is>
-          <t>G600</t>
+          <t>G400</t>
         </is>
       </c>
       <c r="F13" s="8" t="n"/>
@@ -1310,12 +1310,12 @@
       <c r="L13" s="8" t="n"/>
       <c r="M13" s="9" t="inlineStr">
         <is>
-          <t>Abattitore</t>
+          <t>Screw Conveyor</t>
         </is>
       </c>
       <c r="N13" s="9" t="inlineStr">
         <is>
-          <t>Abattitore</t>
+          <t>Screw Conveyor</t>
         </is>
       </c>
       <c r="O13" s="8" t="n"/>
@@ -1349,12 +1349,12 @@
         </is>
       </c>
       <c r="C14" s="8" t="n">
-        <v>710</v>
+        <v>600</v>
       </c>
       <c r="D14" s="8" t="inlineStr"/>
       <c r="E14" s="12" t="inlineStr">
         <is>
-          <t>G710</t>
+          <t>G600</t>
         </is>
       </c>
       <c r="F14" s="8" t="n"/>
@@ -1366,12 +1366,12 @@
       <c r="L14" s="8" t="n"/>
       <c r="M14" s="9" t="inlineStr">
         <is>
-          <t>Pompa</t>
+          <t>Abattitore</t>
         </is>
       </c>
       <c r="N14" s="9" t="inlineStr">
         <is>
-          <t>Pompa a Cavità progressiva</t>
+          <t>Abattitore</t>
         </is>
       </c>
       <c r="O14" s="8" t="n"/>
@@ -1405,12 +1405,12 @@
         </is>
       </c>
       <c r="C15" s="8" t="n">
-        <v>720</v>
+        <v>710</v>
       </c>
       <c r="D15" s="8" t="inlineStr"/>
       <c r="E15" s="12" t="inlineStr">
         <is>
-          <t>G720</t>
+          <t>G710</t>
         </is>
       </c>
       <c r="F15" s="8" t="n"/>
@@ -1422,12 +1422,12 @@
       <c r="L15" s="8" t="n"/>
       <c r="M15" s="9" t="inlineStr">
         <is>
-          <t>FiltroPressa</t>
+          <t>Pompa</t>
         </is>
       </c>
       <c r="N15" s="9" t="inlineStr">
         <is>
-          <t>Filtropressa</t>
+          <t>Pompa a Cavità progressiva</t>
         </is>
       </c>
       <c r="O15" s="8" t="n"/>
@@ -1461,12 +1461,12 @@
         </is>
       </c>
       <c r="C16" s="8" t="n">
-        <v>810</v>
+        <v>720</v>
       </c>
       <c r="D16" s="8" t="inlineStr"/>
       <c r="E16" s="12" t="inlineStr">
         <is>
-          <t>G810</t>
+          <t>G720</t>
         </is>
       </c>
       <c r="F16" s="8" t="n"/>
@@ -1478,12 +1478,12 @@
       <c r="L16" s="8" t="n"/>
       <c r="M16" s="9" t="inlineStr">
         <is>
-          <t>Pompa</t>
+          <t>FiltroPressa</t>
         </is>
       </c>
       <c r="N16" s="9" t="inlineStr">
         <is>
-          <t>Pompa dosatrice</t>
+          <t>Filtropressa</t>
         </is>
       </c>
       <c r="O16" s="8" t="n"/>
@@ -1517,12 +1517,12 @@
         </is>
       </c>
       <c r="C17" s="8" t="n">
-        <v>920</v>
+        <v>810</v>
       </c>
       <c r="D17" s="8" t="inlineStr"/>
       <c r="E17" s="12" t="inlineStr">
         <is>
-          <t>G920</t>
+          <t>G810</t>
         </is>
       </c>
       <c r="F17" s="8" t="n"/>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="N17" s="9" t="inlineStr">
         <is>
-          <t>Pompa chiller</t>
+          <t>Pompa dosatrice</t>
         </is>
       </c>
       <c r="O17" s="8" t="n"/>
@@ -1573,12 +1573,12 @@
         </is>
       </c>
       <c r="C18" s="8" t="n">
-        <v>940</v>
+        <v>920</v>
       </c>
       <c r="D18" s="8" t="inlineStr"/>
       <c r="E18" s="12" t="inlineStr">
         <is>
-          <t>G940</t>
+          <t>G920</t>
         </is>
       </c>
       <c r="F18" s="8" t="n"/>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="N18" s="9" t="inlineStr">
         <is>
-          <t>Pompa dosatrice</t>
+          <t>Pompa chiller</t>
         </is>
       </c>
       <c r="O18" s="8" t="n"/>
@@ -1625,16 +1625,16 @@
       </c>
       <c r="B19" s="8" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>G</t>
         </is>
       </c>
       <c r="C19" s="8" t="n">
-        <v>850</v>
+        <v>940</v>
       </c>
       <c r="D19" s="8" t="inlineStr"/>
       <c r="E19" s="12" t="inlineStr">
         <is>
-          <t>H850</t>
+          <t>G940</t>
         </is>
       </c>
       <c r="F19" s="8" t="n"/>
@@ -1646,12 +1646,12 @@
       <c r="L19" s="8" t="n"/>
       <c r="M19" s="9" t="inlineStr">
         <is>
-          <t>Heater</t>
+          <t>Pompa</t>
         </is>
       </c>
       <c r="N19" s="9" t="inlineStr">
         <is>
-          <t>Riscaldatore</t>
+          <t>Pompa dosatrice</t>
         </is>
       </c>
       <c r="O19" s="8" t="n"/>
@@ -1681,16 +1681,16 @@
       </c>
       <c r="B20" s="8" t="inlineStr">
         <is>
-          <t>HE</t>
+          <t>H</t>
         </is>
       </c>
       <c r="C20" s="8" t="n">
-        <v>900</v>
+        <v>850</v>
       </c>
       <c r="D20" s="8" t="inlineStr"/>
       <c r="E20" s="12" t="inlineStr">
         <is>
-          <t>HE900</t>
+          <t>H850</t>
         </is>
       </c>
       <c r="F20" s="8" t="n"/>
@@ -1702,12 +1702,12 @@
       <c r="L20" s="8" t="n"/>
       <c r="M20" s="9" t="inlineStr">
         <is>
-          <t>Heater Exchanger</t>
+          <t>Heater</t>
         </is>
       </c>
       <c r="N20" s="9" t="inlineStr">
         <is>
-          <t>Heater Exchanger</t>
+          <t>Riscaldatore</t>
         </is>
       </c>
       <c r="O20" s="8" t="n"/>
@@ -1741,12 +1741,12 @@
         </is>
       </c>
       <c r="C21" s="8" t="n">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="D21" s="8" t="inlineStr"/>
       <c r="E21" s="12" t="inlineStr">
         <is>
-          <t>HE905</t>
+          <t>HE900</t>
         </is>
       </c>
       <c r="F21" s="8" t="n"/>
@@ -2516,15 +2516,23 @@
       <c r="J35" s="8" t="n"/>
       <c r="K35" s="8" t="n"/>
       <c r="L35" s="8" t="n"/>
-      <c r="M35" s="9" t="inlineStr"/>
-      <c r="N35" s="9" t="n"/>
+      <c r="M35" s="9" t="inlineStr">
+        <is>
+          <t>Ball Valve with Pneumatic actuator</t>
+        </is>
+      </c>
+      <c r="N35" s="9" t="inlineStr"/>
       <c r="O35" s="8" t="n"/>
       <c r="P35" s="9" t="n"/>
       <c r="Q35" s="10" t="n"/>
       <c r="R35" s="8" t="n"/>
       <c r="S35" s="8" t="n"/>
       <c r="T35" s="8" t="n"/>
-      <c r="U35" s="8" t="n"/>
+      <c r="U35" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
       <c r="V35" s="8" t="n"/>
       <c r="W35" s="8" t="n"/>
       <c r="X35" s="9" t="n"/>
@@ -2564,7 +2572,11 @@
       <c r="J36" s="8" t="n"/>
       <c r="K36" s="8" t="n"/>
       <c r="L36" s="8" t="n"/>
-      <c r="M36" s="9" t="inlineStr"/>
+      <c r="M36" s="9" t="inlineStr">
+        <is>
+          <t>Ball Valve with Pneumatic actuator  1212</t>
+        </is>
+      </c>
       <c r="N36" s="9" t="n"/>
       <c r="O36" s="8" t="n"/>
       <c r="P36" s="9" t="n"/>
@@ -2612,15 +2624,23 @@
       <c r="J37" s="8" t="n"/>
       <c r="K37" s="8" t="n"/>
       <c r="L37" s="8" t="n"/>
-      <c r="M37" s="9" t="inlineStr"/>
-      <c r="N37" s="9" t="n"/>
+      <c r="M37" s="9" t="inlineStr">
+        <is>
+          <t>Ball Valve with Pneumatic actuator</t>
+        </is>
+      </c>
+      <c r="N37" s="9" t="inlineStr"/>
       <c r="O37" s="8" t="n"/>
       <c r="P37" s="9" t="n"/>
       <c r="Q37" s="10" t="n"/>
       <c r="R37" s="8" t="n"/>
       <c r="S37" s="8" t="n"/>
       <c r="T37" s="8" t="n"/>
-      <c r="U37" s="8" t="n"/>
+      <c r="U37" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V37" s="8" t="n"/>
       <c r="W37" s="8" t="n"/>
       <c r="X37" s="9" t="n"/>
@@ -2660,7 +2680,11 @@
       <c r="J38" s="8" t="n"/>
       <c r="K38" s="8" t="n"/>
       <c r="L38" s="8" t="n"/>
-      <c r="M38" s="9" t="inlineStr"/>
+      <c r="M38" s="9" t="inlineStr">
+        <is>
+          <t>Ball Valve with Pneumatic actuator</t>
+        </is>
+      </c>
       <c r="N38" s="9" t="n"/>
       <c r="O38" s="8" t="n"/>
       <c r="P38" s="9" t="n"/>

</xml_diff>